<commit_message>
Update to Hierarchy from 2/24/2020 meeting
</commit_message>
<xml_diff>
--- a/OnSeason/Macomb/RAW.xlsx
+++ b/OnSeason/Macomb/RAW.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Scouting\Documents\2020Scouting\Pre-Season\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Scouting\Documents\2020Scouting\OnSeason\Macomb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61591329-49C0-4BA7-9F0B-2CBD0814F742}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9177228-9AFC-4976-B96C-50E0341C5A21}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{79F0924D-00AD-40AC-B418-85808285862A}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet2" sheetId="5" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_3" localSheetId="0" hidden="1">Sheet2!$A$1:$AR$7</definedName>
+    <definedName name="ExternalData_3" localSheetId="0" hidden="1">Sheet2!$A$1:$AR$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>File name</t>
   </si>
@@ -177,42 +177,6 @@
   </si>
   <si>
     <t>Team#.Question007</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>01</t>
-  </si>
-  <si>
-    <t>01|02|03</t>
-  </si>
-  <si>
-    <t>01|02|03|04</t>
-  </si>
-  <si>
-    <t>B2</t>
-  </si>
-  <si>
-    <t>01|02|03|04|05</t>
-  </si>
-  <si>
-    <t>01|02</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>B1</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>B3</t>
   </si>
 </sst>
 </file>
@@ -368,8 +332,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{75453F21-F838-432F-B289-153B9FF87A19}" name="_MJ2" displayName="_MJ2" ref="A1:AR7" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:AR7" xr:uid="{E6D22501-77D3-4AAE-A57B-BEF0423633B0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{75453F21-F838-432F-B289-153B9FF87A19}" name="_MJ2" displayName="_MJ2" ref="A1:AR2" tableType="queryTable" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A1:AR2" xr:uid="{E6D22501-77D3-4AAE-A57B-BEF0423633B0}"/>
   <tableColumns count="44">
     <tableColumn id="1" xr3:uid="{58DF038D-918F-4F86-A1E3-09ADB3598F1E}" uniqueName="1" name="File name" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{61EE88DA-E634-4DD8-B74B-C9D8E187DD4D}" uniqueName="2" name="Alliance 2-Ball Trench.Question013" queryTableFieldId="2" dataDxfId="14"/>
@@ -717,10 +681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62784BB4-501E-400B-A6E9-98C2C6A00C48}">
-  <dimension ref="A1:AR7"/>
+  <dimension ref="A1:AR2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:AR7"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -888,643 +852,21 @@
       </c>
     </row>
     <row r="2" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>4</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q2">
-        <v>1</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AC2">
-        <v>0</v>
-      </c>
-      <c r="AD2">
-        <v>0</v>
-      </c>
-      <c r="AE2">
-        <v>1</v>
-      </c>
-      <c r="AF2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AH2">
-        <v>2</v>
-      </c>
-      <c r="AI2">
-        <v>1</v>
-      </c>
-      <c r="AJ2">
-        <v>2</v>
-      </c>
-      <c r="AK2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AL2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AM2">
-        <v>1</v>
-      </c>
-      <c r="AN2">
-        <v>1</v>
-      </c>
-      <c r="AO2">
-        <v>0</v>
-      </c>
-      <c r="AP2">
-        <v>2</v>
-      </c>
-      <c r="AQ2">
-        <v>1</v>
-      </c>
-      <c r="AR2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E3">
-        <v>4</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="X3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AC3">
-        <v>0</v>
-      </c>
-      <c r="AD3">
-        <v>0</v>
-      </c>
-      <c r="AE3">
-        <v>1</v>
-      </c>
-      <c r="AF3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AG3">
-        <v>1</v>
-      </c>
-      <c r="AH3">
-        <v>0</v>
-      </c>
-      <c r="AI3">
-        <v>1</v>
-      </c>
-      <c r="AJ3">
-        <v>1</v>
-      </c>
-      <c r="AK3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AL3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AM3">
-        <v>1</v>
-      </c>
-      <c r="AN3">
-        <v>2</v>
-      </c>
-      <c r="AO3">
-        <v>0</v>
-      </c>
-      <c r="AP3">
-        <v>3</v>
-      </c>
-      <c r="AQ3">
-        <v>0</v>
-      </c>
-      <c r="AR3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>2</v>
-      </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="X4" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA4">
-        <v>1</v>
-      </c>
-      <c r="AC4">
-        <v>0</v>
-      </c>
-      <c r="AD4">
-        <v>0</v>
-      </c>
-      <c r="AE4">
-        <v>1</v>
-      </c>
-      <c r="AF4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AH4">
-        <v>2</v>
-      </c>
-      <c r="AI4">
-        <v>1</v>
-      </c>
-      <c r="AJ4">
-        <v>0</v>
-      </c>
-      <c r="AK4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="AL4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AM4">
-        <v>1</v>
-      </c>
-      <c r="AN4">
-        <v>1</v>
-      </c>
-      <c r="AO4">
-        <v>0</v>
-      </c>
-      <c r="AP4">
-        <v>9</v>
-      </c>
-      <c r="AQ4">
-        <v>1</v>
-      </c>
-      <c r="AR4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q5">
-        <v>1</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="V5">
-        <v>1</v>
-      </c>
-      <c r="W5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="X5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB5">
-        <v>1</v>
-      </c>
-      <c r="AC5">
-        <v>0</v>
-      </c>
-      <c r="AD5">
-        <v>0</v>
-      </c>
-      <c r="AE5">
-        <v>1</v>
-      </c>
-      <c r="AF5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AH5">
-        <v>1</v>
-      </c>
-      <c r="AJ5">
-        <v>0</v>
-      </c>
-      <c r="AK5" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AM5">
-        <v>1</v>
-      </c>
-      <c r="AN5">
-        <v>0</v>
-      </c>
-      <c r="AO5">
-        <v>1</v>
-      </c>
-      <c r="AP5">
-        <v>1</v>
-      </c>
-      <c r="AQ5">
-        <v>8</v>
-      </c>
-      <c r="AR5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>1</v>
-      </c>
-      <c r="M6">
-        <v>1</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="T6" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="W6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="X6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA6">
-        <v>1</v>
-      </c>
-      <c r="AC6">
-        <v>0</v>
-      </c>
-      <c r="AD6">
-        <v>0</v>
-      </c>
-      <c r="AE6">
-        <v>1</v>
-      </c>
-      <c r="AF6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AH6">
-        <v>0</v>
-      </c>
-      <c r="AJ6">
-        <v>1</v>
-      </c>
-      <c r="AK6" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AL6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AM6">
-        <v>2</v>
-      </c>
-      <c r="AN6">
-        <v>1</v>
-      </c>
-      <c r="AO6">
-        <v>1</v>
-      </c>
-      <c r="AP6">
-        <v>7</v>
-      </c>
-      <c r="AQ6">
-        <v>1</v>
-      </c>
-      <c r="AR6">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>1</v>
-      </c>
-      <c r="M7">
-        <v>1</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="R7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="S7" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="T7" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="U7" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="W7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="X7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z7" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AA7">
-        <v>1</v>
-      </c>
-      <c r="AB7">
-        <v>1</v>
-      </c>
-      <c r="AC7">
-        <v>0</v>
-      </c>
-      <c r="AD7">
-        <v>0</v>
-      </c>
-      <c r="AE7">
-        <v>1</v>
-      </c>
-      <c r="AF7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AH7">
-        <v>1</v>
-      </c>
-      <c r="AI7">
-        <v>1</v>
-      </c>
-      <c r="AJ7">
-        <v>0</v>
-      </c>
-      <c r="AK7" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AL7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AM7">
-        <v>1</v>
-      </c>
-      <c r="AN7">
-        <v>1</v>
-      </c>
-      <c r="AO7">
-        <v>2</v>
-      </c>
-      <c r="AP7">
-        <v>8</v>
-      </c>
-      <c r="AQ7">
-        <v>3</v>
-      </c>
-      <c r="AR7">
-        <v>4</v>
-      </c>
+      <c r="B2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AF2" s="1"/>
+      <c r="AK2" s="1"/>
+      <c r="AL2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>